<commit_message>
Actualizando avances en lista de chequeo
</commit_message>
<xml_diff>
--- a/Documentacion/Proyecto - Lista de Chequeo.xlsx
+++ b/Documentacion/Proyecto - Lista de Chequeo.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matrix\Downloads\Usac 2020\2 Semestre\PROYECTOS\Proyecto2020_SergioDePaz_201221022\Proyecto_SergioDePaz_201221022\Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matrix\Downloads\Usac 2020\2 Semestre\PROYECTOS\Proyecto2020_SergioDePaz_201221022\Proyecto_SergioDePaz_201221022\Proyecto_SergioDePaz_201221022\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="19560" windowHeight="8235"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="19560" windowHeight="8235"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$A$1:$I$19</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="70">
   <si>
     <t>1.1</t>
   </si>
@@ -268,7 +267,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0\ [$GTQ]"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -337,6 +336,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -962,7 +969,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1218,6 +1225,54 @@
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0" hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0" hidden="1"/>
@@ -1243,54 +1298,6 @@
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0" hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0" hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0" hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0" hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0" hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0" hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0" hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0" hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0" hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0" hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0" hidden="1"/>
@@ -1307,6 +1314,8 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0" hidden="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1908,8 +1917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1927,30 +1936,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="86" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="99"/>
-      <c r="C1" s="99"/>
-      <c r="D1" s="99"/>
-      <c r="E1" s="99"/>
-      <c r="F1" s="99"/>
-      <c r="G1" s="99"/>
-      <c r="H1" s="99"/>
-      <c r="I1" s="99"/>
+      <c r="B1" s="86"/>
+      <c r="C1" s="86"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="105" t="s">
+      <c r="A2" s="97" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="105"/>
-      <c r="C2" s="105"/>
-      <c r="D2" s="105"/>
-      <c r="E2" s="105"/>
-      <c r="F2" s="105"/>
-      <c r="G2" s="105"/>
-      <c r="H2" s="105"/>
-      <c r="I2" s="105"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="41" t="s">
@@ -1968,62 +1977,62 @@
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="103" t="s">
+      <c r="A5" s="95" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="103"/>
-      <c r="C5" s="104" t="s">
+      <c r="B5" s="95"/>
+      <c r="C5" s="96" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="104"/>
+      <c r="D5" s="96"/>
       <c r="E5" s="43"/>
       <c r="F5" s="44"/>
-      <c r="G5" s="107"/>
-      <c r="H5" s="107"/>
-      <c r="I5" s="107"/>
+      <c r="G5" s="99"/>
+      <c r="H5" s="99"/>
+      <c r="I5" s="99"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="89">
+      <c r="A6" s="104">
         <v>201221022</v>
       </c>
-      <c r="B6" s="89"/>
-      <c r="C6" s="89" t="s">
+      <c r="B6" s="104"/>
+      <c r="C6" s="104" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="89"/>
+      <c r="D6" s="104"/>
       <c r="E6" s="43"/>
       <c r="F6" s="45"/>
-      <c r="G6" s="108"/>
-      <c r="H6" s="108"/>
-      <c r="I6" s="108"/>
+      <c r="G6" s="100"/>
+      <c r="H6" s="100"/>
+      <c r="I6" s="100"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="89"/>
-      <c r="B7" s="89"/>
-      <c r="C7" s="89"/>
-      <c r="D7" s="89"/>
+      <c r="A7" s="104"/>
+      <c r="B7" s="104"/>
+      <c r="C7" s="104"/>
+      <c r="D7" s="104"/>
       <c r="E7" s="43"/>
       <c r="F7" s="46"/>
-      <c r="G7" s="108"/>
-      <c r="H7" s="108"/>
-      <c r="I7" s="108"/>
+      <c r="G7" s="100"/>
+      <c r="H7" s="100"/>
+      <c r="I7" s="100"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="89"/>
-      <c r="B8" s="89"/>
-      <c r="C8" s="89"/>
-      <c r="D8" s="89"/>
+      <c r="A8" s="104"/>
+      <c r="B8" s="104"/>
+      <c r="C8" s="104"/>
+      <c r="D8" s="104"/>
       <c r="E8" s="43"/>
       <c r="F8" s="46"/>
-      <c r="G8" s="108"/>
-      <c r="H8" s="108"/>
-      <c r="I8" s="108"/>
+      <c r="G8" s="100"/>
+      <c r="H8" s="100"/>
+      <c r="I8" s="100"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="91"/>
-      <c r="B9" s="91"/>
-      <c r="C9" s="90"/>
-      <c r="D9" s="90"/>
+      <c r="A9" s="106"/>
+      <c r="B9" s="106"/>
+      <c r="C9" s="105"/>
+      <c r="D9" s="105"/>
     </row>
     <row r="10" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="29" t="s">
@@ -2036,11 +2045,11 @@
         <v>16</v>
       </c>
       <c r="C11" s="38"/>
-      <c r="D11" s="100" t="s">
+      <c r="D11" s="89" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="101"/>
-      <c r="F11" s="102"/>
+      <c r="E11" s="90"/>
+      <c r="F11" s="91"/>
       <c r="G11" s="40" t="s">
         <v>44</v>
       </c>
@@ -2055,15 +2064,15 @@
       <c r="A12" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="94" t="s">
+      <c r="B12" s="87" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="95"/>
-      <c r="D12" s="96" t="s">
+      <c r="C12" s="88"/>
+      <c r="D12" s="92" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="97"/>
-      <c r="F12" s="98"/>
+      <c r="E12" s="93"/>
+      <c r="F12" s="94"/>
       <c r="G12" s="7" t="s">
         <v>49</v>
       </c>
@@ -2082,11 +2091,11 @@
         <v>33</v>
       </c>
       <c r="C13" s="34"/>
-      <c r="D13" s="96" t="s">
+      <c r="D13" s="92" t="s">
         <v>50</v>
       </c>
-      <c r="E13" s="97"/>
-      <c r="F13" s="98"/>
+      <c r="E13" s="93"/>
+      <c r="F13" s="94"/>
       <c r="G13" s="7" t="s">
         <v>49</v>
       </c>
@@ -2101,15 +2110,15 @@
       <c r="A14" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="94" t="s">
+      <c r="B14" s="87" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="95"/>
-      <c r="D14" s="96" t="s">
+      <c r="C14" s="88"/>
+      <c r="D14" s="92" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="97"/>
-      <c r="F14" s="98"/>
+      <c r="E14" s="93"/>
+      <c r="F14" s="94"/>
       <c r="G14" s="7" t="s">
         <v>49</v>
       </c>
@@ -2128,16 +2137,16 @@
         <v>32</v>
       </c>
       <c r="C15" s="34"/>
-      <c r="D15" s="94" t="s">
+      <c r="D15" s="87" t="s">
         <v>51</v>
       </c>
-      <c r="E15" s="106"/>
-      <c r="F15" s="95"/>
+      <c r="E15" s="98"/>
+      <c r="F15" s="88"/>
       <c r="G15" s="7" t="s">
         <v>49</v>
       </c>
       <c r="H15" s="48">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="I15" s="6"/>
     </row>
@@ -2149,49 +2158,51 @@
         <v>45</v>
       </c>
       <c r="C16" s="34"/>
-      <c r="D16" s="96" t="s">
+      <c r="D16" s="92" t="s">
         <v>52</v>
       </c>
-      <c r="E16" s="97"/>
-      <c r="F16" s="98"/>
+      <c r="E16" s="93"/>
+      <c r="F16" s="94"/>
       <c r="G16" s="7" t="s">
         <v>49</v>
       </c>
       <c r="H16" s="48">
-        <v>0.75</v>
-      </c>
-      <c r="I16" s="6"/>
+        <v>1</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="94" t="s">
+      <c r="B17" s="87" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="95"/>
-      <c r="D17" s="94" t="s">
+      <c r="C17" s="88"/>
+      <c r="D17" s="87" t="s">
         <v>60</v>
       </c>
-      <c r="E17" s="106"/>
-      <c r="F17" s="95"/>
+      <c r="E17" s="98"/>
+      <c r="F17" s="88"/>
       <c r="G17" s="7" t="s">
         <v>49</v>
       </c>
       <c r="H17" s="48">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="I17" s="6"/>
     </row>
     <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10"/>
-      <c r="B18" s="92"/>
-      <c r="C18" s="93"/>
-      <c r="D18" s="86"/>
-      <c r="E18" s="87"/>
-      <c r="F18" s="88"/>
+      <c r="B18" s="107"/>
+      <c r="C18" s="108"/>
+      <c r="D18" s="101"/>
+      <c r="E18" s="102"/>
+      <c r="F18" s="103"/>
       <c r="G18" s="12"/>
-      <c r="H18" s="13"/>
+      <c r="H18" s="114"/>
       <c r="I18" s="11"/>
     </row>
     <row r="21" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
@@ -2407,7 +2418,9 @@
       <c r="G34" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="H34" s="7"/>
+      <c r="H34" s="113">
+        <v>0.3</v>
+      </c>
       <c r="I34" s="14"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -2426,7 +2439,9 @@
       <c r="G35" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="H35" s="7"/>
+      <c r="H35" s="113">
+        <v>0.3</v>
+      </c>
       <c r="I35" s="14"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -2445,7 +2460,9 @@
       <c r="G36" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="H36" s="7"/>
+      <c r="H36" s="113">
+        <v>0.3</v>
+      </c>
       <c r="I36" s="14"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -2464,7 +2481,9 @@
       <c r="G37" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="H37" s="7"/>
+      <c r="H37" s="113">
+        <v>0.3</v>
+      </c>
       <c r="I37" s="14"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -2528,6 +2547,18 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="D16:F16"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B17:C17"/>
@@ -2544,18 +2575,6 @@
     <mergeCell ref="G6:I6"/>
     <mergeCell ref="G7:I7"/>
     <mergeCell ref="G8:I8"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="D16:F16"/>
   </mergeCells>
   <conditionalFormatting sqref="A26:F26 A33:B36 F25 D18 D11:E13 B15:B18 A13:A18 I11:I18 A29:F29 I26:I29 F32:F36 I33:I40 B27:F28 A37:F40">
     <cfRule type="expression" dxfId="10" priority="35" stopIfTrue="1">
@@ -2603,7 +2622,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Actualizacion de listad de chequeo
</commit_message>
<xml_diff>
--- a/Documentacion/Proyecto - Lista de Chequeo.xlsx
+++ b/Documentacion/Proyecto - Lista de Chequeo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="19560" windowHeight="8235"/>
+    <workbookView xWindow="3720" yWindow="0" windowWidth="19560" windowHeight="8235"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -969,7 +969,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1192,7 +1192,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0" hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0" hidden="1"/>
@@ -1225,17 +1224,56 @@
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0" hidden="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0" hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0" hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0" hidden="1"/>
@@ -1246,18 +1284,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0" hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0" hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0" hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0" hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1273,31 +1299,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0" hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0" hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0" hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0" hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0" hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0" hidden="1"/>
@@ -1314,8 +1315,8 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0" hidden="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1917,8 +1918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1936,30 +1937,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="86"/>
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
+      <c r="G1" s="100"/>
+      <c r="H1" s="100"/>
+      <c r="I1" s="100"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="97" t="s">
+      <c r="A2" s="106" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
+      <c r="B2" s="106"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="106"/>
+      <c r="F2" s="106"/>
+      <c r="G2" s="106"/>
+      <c r="H2" s="106"/>
+      <c r="I2" s="106"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="41" t="s">
@@ -1977,62 +1978,62 @@
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="95" t="s">
+      <c r="A5" s="104" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="95"/>
-      <c r="C5" s="96" t="s">
+      <c r="B5" s="104"/>
+      <c r="C5" s="105" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="96"/>
+      <c r="D5" s="105"/>
       <c r="E5" s="43"/>
       <c r="F5" s="44"/>
-      <c r="G5" s="99"/>
-      <c r="H5" s="99"/>
-      <c r="I5" s="99"/>
+      <c r="G5" s="108"/>
+      <c r="H5" s="108"/>
+      <c r="I5" s="108"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="104">
+      <c r="A6" s="90">
         <v>201221022</v>
       </c>
-      <c r="B6" s="104"/>
-      <c r="C6" s="104" t="s">
+      <c r="B6" s="90"/>
+      <c r="C6" s="90" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="104"/>
+      <c r="D6" s="90"/>
       <c r="E6" s="43"/>
       <c r="F6" s="45"/>
-      <c r="G6" s="100"/>
-      <c r="H6" s="100"/>
-      <c r="I6" s="100"/>
+      <c r="G6" s="109"/>
+      <c r="H6" s="109"/>
+      <c r="I6" s="109"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="104"/>
-      <c r="B7" s="104"/>
-      <c r="C7" s="104"/>
-      <c r="D7" s="104"/>
+      <c r="A7" s="90"/>
+      <c r="B7" s="90"/>
+      <c r="C7" s="90"/>
+      <c r="D7" s="90"/>
       <c r="E7" s="43"/>
       <c r="F7" s="46"/>
-      <c r="G7" s="100"/>
-      <c r="H7" s="100"/>
-      <c r="I7" s="100"/>
+      <c r="G7" s="109"/>
+      <c r="H7" s="109"/>
+      <c r="I7" s="109"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="104"/>
-      <c r="B8" s="104"/>
-      <c r="C8" s="104"/>
-      <c r="D8" s="104"/>
+      <c r="A8" s="90"/>
+      <c r="B8" s="90"/>
+      <c r="C8" s="90"/>
+      <c r="D8" s="90"/>
       <c r="E8" s="43"/>
       <c r="F8" s="46"/>
-      <c r="G8" s="100"/>
-      <c r="H8" s="100"/>
-      <c r="I8" s="100"/>
+      <c r="G8" s="109"/>
+      <c r="H8" s="109"/>
+      <c r="I8" s="109"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="106"/>
-      <c r="B9" s="106"/>
-      <c r="C9" s="105"/>
-      <c r="D9" s="105"/>
+      <c r="A9" s="92"/>
+      <c r="B9" s="92"/>
+      <c r="C9" s="91"/>
+      <c r="D9" s="91"/>
     </row>
     <row r="10" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="29" t="s">
@@ -2045,11 +2046,11 @@
         <v>16</v>
       </c>
       <c r="C11" s="38"/>
-      <c r="D11" s="89" t="s">
+      <c r="D11" s="101" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="90"/>
-      <c r="F11" s="91"/>
+      <c r="E11" s="102"/>
+      <c r="F11" s="103"/>
       <c r="G11" s="40" t="s">
         <v>44</v>
       </c>
@@ -2064,15 +2065,15 @@
       <c r="A12" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="87" t="s">
+      <c r="B12" s="95" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="88"/>
-      <c r="D12" s="92" t="s">
+      <c r="C12" s="96"/>
+      <c r="D12" s="97" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="93"/>
-      <c r="F12" s="94"/>
+      <c r="E12" s="98"/>
+      <c r="F12" s="99"/>
       <c r="G12" s="7" t="s">
         <v>49</v>
       </c>
@@ -2091,11 +2092,11 @@
         <v>33</v>
       </c>
       <c r="C13" s="34"/>
-      <c r="D13" s="92" t="s">
+      <c r="D13" s="97" t="s">
         <v>50</v>
       </c>
-      <c r="E13" s="93"/>
-      <c r="F13" s="94"/>
+      <c r="E13" s="98"/>
+      <c r="F13" s="99"/>
       <c r="G13" s="7" t="s">
         <v>49</v>
       </c>
@@ -2110,15 +2111,15 @@
       <c r="A14" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="87" t="s">
+      <c r="B14" s="95" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="88"/>
-      <c r="D14" s="92" t="s">
+      <c r="C14" s="96"/>
+      <c r="D14" s="97" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="93"/>
-      <c r="F14" s="94"/>
+      <c r="E14" s="98"/>
+      <c r="F14" s="99"/>
       <c r="G14" s="7" t="s">
         <v>49</v>
       </c>
@@ -2137,11 +2138,11 @@
         <v>32</v>
       </c>
       <c r="C15" s="34"/>
-      <c r="D15" s="87" t="s">
+      <c r="D15" s="95" t="s">
         <v>51</v>
       </c>
-      <c r="E15" s="98"/>
-      <c r="F15" s="88"/>
+      <c r="E15" s="107"/>
+      <c r="F15" s="96"/>
       <c r="G15" s="7" t="s">
         <v>49</v>
       </c>
@@ -2158,11 +2159,11 @@
         <v>45</v>
       </c>
       <c r="C16" s="34"/>
-      <c r="D16" s="92" t="s">
+      <c r="D16" s="97" t="s">
         <v>52</v>
       </c>
-      <c r="E16" s="93"/>
-      <c r="F16" s="94"/>
+      <c r="E16" s="98"/>
+      <c r="F16" s="99"/>
       <c r="G16" s="7" t="s">
         <v>49</v>
       </c>
@@ -2177,15 +2178,15 @@
       <c r="A17" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="87" t="s">
+      <c r="B17" s="95" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="88"/>
-      <c r="D17" s="87" t="s">
+      <c r="C17" s="96"/>
+      <c r="D17" s="95" t="s">
         <v>60</v>
       </c>
-      <c r="E17" s="98"/>
-      <c r="F17" s="88"/>
+      <c r="E17" s="107"/>
+      <c r="F17" s="96"/>
       <c r="G17" s="7" t="s">
         <v>49</v>
       </c>
@@ -2196,13 +2197,13 @@
     </row>
     <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10"/>
-      <c r="B18" s="107"/>
-      <c r="C18" s="108"/>
-      <c r="D18" s="101"/>
-      <c r="E18" s="102"/>
-      <c r="F18" s="103"/>
+      <c r="B18" s="93"/>
+      <c r="C18" s="94"/>
+      <c r="D18" s="87"/>
+      <c r="E18" s="88"/>
+      <c r="F18" s="89"/>
       <c r="G18" s="12"/>
-      <c r="H18" s="114"/>
+      <c r="H18" s="86"/>
       <c r="I18" s="11"/>
     </row>
     <row r="21" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
@@ -2374,7 +2375,7 @@
       <c r="C32" s="52"/>
       <c r="D32" s="52"/>
       <c r="E32" s="52"/>
-      <c r="F32" s="83" t="s">
+      <c r="F32" s="82" t="s">
         <v>15</v>
       </c>
       <c r="G32" s="53" t="s">
@@ -2383,7 +2384,7 @@
       <c r="H32" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="I32" s="84" t="s">
+      <c r="I32" s="83" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2391,16 +2392,16 @@
       <c r="A33" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="B33" s="79" t="s">
+      <c r="B33" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="C33" s="80"/>
-      <c r="D33" s="80"/>
-      <c r="E33" s="80"/>
-      <c r="F33" s="81"/>
+      <c r="C33" s="79"/>
+      <c r="D33" s="79"/>
+      <c r="E33" s="79"/>
+      <c r="F33" s="80"/>
       <c r="G33" s="50"/>
       <c r="H33" s="50"/>
-      <c r="I33" s="82"/>
+      <c r="I33" s="81"/>
     </row>
     <row r="34" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
@@ -2418,7 +2419,7 @@
       <c r="G34" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="H34" s="113">
+      <c r="H34" s="85">
         <v>0.3</v>
       </c>
       <c r="I34" s="14"/>
@@ -2439,7 +2440,7 @@
       <c r="G35" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="H35" s="113">
+      <c r="H35" s="85">
         <v>0.3</v>
       </c>
       <c r="I35" s="14"/>
@@ -2460,7 +2461,7 @@
       <c r="G36" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="H36" s="113">
+      <c r="H36" s="85">
         <v>0.3</v>
       </c>
       <c r="I36" s="14"/>
@@ -2481,7 +2482,7 @@
       <c r="G37" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="H37" s="113">
+      <c r="H37" s="85">
         <v>0.3</v>
       </c>
       <c r="I37" s="14"/>
@@ -2517,13 +2518,15 @@
       <c r="G39" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="H39" s="77"/>
-      <c r="I39" s="78"/>
+      <c r="H39" s="114">
+        <v>0.1</v>
+      </c>
+      <c r="I39" s="77"/>
     </row>
     <row r="40" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="10"/>
       <c r="B40" s="31"/>
-      <c r="C40" s="85" t="s">
+      <c r="C40" s="84" t="s">
         <v>63</v>
       </c>
       <c r="D40" s="11"/>
@@ -2534,7 +2537,9 @@
       <c r="G40" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="H40" s="12"/>
+      <c r="H40" s="115">
+        <v>0.1</v>
+      </c>
       <c r="I40" s="17"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -2547,18 +2552,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="D16:F16"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B17:C17"/>
@@ -2575,6 +2568,18 @@
     <mergeCell ref="G6:I6"/>
     <mergeCell ref="G7:I7"/>
     <mergeCell ref="G8:I8"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="D16:F16"/>
   </mergeCells>
   <conditionalFormatting sqref="A26:F26 A33:B36 F25 D18 D11:E13 B15:B18 A13:A18 I11:I18 A29:F29 I26:I29 F32:F36 I33:I40 B27:F28 A37:F40">
     <cfRule type="expression" dxfId="10" priority="35" stopIfTrue="1">
@@ -2760,11 +2765,11 @@
         <v>54</v>
       </c>
       <c r="D11" s="57"/>
-      <c r="E11" s="109" t="s">
+      <c r="E11" s="110" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="110"/>
-      <c r="G11" s="111"/>
+      <c r="F11" s="111"/>
+      <c r="G11" s="112"/>
       <c r="H11" s="53" t="s">
         <v>44</v>
       </c>
@@ -2785,15 +2790,15 @@
       <c r="B12" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="112" t="s">
+      <c r="C12" s="113" t="s">
         <v>57</v>
       </c>
-      <c r="D12" s="112"/>
-      <c r="E12" s="112" t="s">
+      <c r="D12" s="113"/>
+      <c r="E12" s="113" t="s">
         <v>58</v>
       </c>
-      <c r="F12" s="112"/>
-      <c r="G12" s="112"/>
+      <c r="F12" s="113"/>
+      <c r="G12" s="113"/>
       <c r="H12" s="58" t="s">
         <v>49</v>
       </c>

</xml_diff>